<commit_message>
Substract only 10 GW
</commit_message>
<xml_diff>
--- a/Code/Prosumage_Opt/Dieter_Module/DIETER_PROSUMOD_MCP/data_input.xlsx
+++ b/Code/Prosumage_Opt/Dieter_Module/DIETER_PROSUMOD_MCP/data_input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">storage!$A$5:$M$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Technologies!$A$5:$U$16</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -38,7 +38,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="V11" authorId="0" shapeId="0">
+    <comment ref="V11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V13" authorId="0" shapeId="0">
+    <comment ref="V13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1422,11 +1422,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1753,7 +1753,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1789,7 +1789,7 @@
         <xdr:cNvPr id="2" name="Grafik 1" descr="Creative Commons Lizenzvertrag">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1801,7 +1801,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1821,7 +1821,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1836,9 +1836,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1876,9 +1876,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1910,10 +1910,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1945,10 +1944,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2121,7 +2119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B2"/>
   <sheetViews>
@@ -2129,9 +2127,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2143,7 +2141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle10"/>
   <dimension ref="A1:AA125"/>
   <sheetViews>
@@ -2151,7 +2149,7 @@
       <selection sqref="A1:XFD125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="13"/>
     <col min="3" max="6" width="14" style="13" customWidth="1"/>
@@ -2163,7 +2161,7 @@
     <col min="19" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="A4" s="13" t="s">
         <v>26</v>
       </c>
@@ -2331,7 +2329,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="38" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="38" customFormat="1" ht="30.75" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>45</v>
       </c>
@@ -2399,7 +2397,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27">
       <c r="A6" s="13" t="s">
         <v>130</v>
       </c>
@@ -2446,7 +2444,7 @@
       <c r="Y6" s="24"/>
       <c r="AA6" s="24"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27">
       <c r="A7" s="13" t="s">
         <v>130</v>
       </c>
@@ -2508,7 +2506,7 @@
       <c r="Y7" s="24"/>
       <c r="AA7" s="24"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27">
       <c r="A8" s="13" t="s">
         <v>130</v>
       </c>
@@ -2562,7 +2560,7 @@
       <c r="Y8" s="24"/>
       <c r="AA8" s="24"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27">
       <c r="A9" s="13" t="s">
         <v>130</v>
       </c>
@@ -2619,7 +2617,7 @@
       <c r="Y9" s="24"/>
       <c r="AA9" s="24"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27">
       <c r="A10" s="13" t="s">
         <v>130</v>
       </c>
@@ -2672,7 +2670,7 @@
       <c r="Y10" s="24"/>
       <c r="AA10" s="24"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27">
       <c r="A11" s="13" t="s">
         <v>130</v>
       </c>
@@ -2728,7 +2726,7 @@
       <c r="Y11" s="24"/>
       <c r="AA11" s="24"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27">
       <c r="A12" s="13" t="s">
         <v>130</v>
       </c>
@@ -2779,7 +2777,7 @@
       <c r="Y12" s="24"/>
       <c r="AA12" s="24"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27">
       <c r="A13" s="13" t="s">
         <v>130</v>
       </c>
@@ -2830,7 +2828,7 @@
       <c r="Y13" s="24"/>
       <c r="AA13" s="24"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27">
       <c r="A14" s="13" t="s">
         <v>130</v>
       </c>
@@ -2887,7 +2885,7 @@
       <c r="Y14" s="24"/>
       <c r="AA14" s="24"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27">
       <c r="A15" s="13" t="s">
         <v>130</v>
       </c>
@@ -2947,7 +2945,7 @@
       <c r="Y15" s="24"/>
       <c r="AA15" s="24"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27">
       <c r="A16" s="13" t="s">
         <v>130</v>
       </c>
@@ -2992,7 +2990,7 @@
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="13" t="s">
         <v>130</v>
       </c>
@@ -3052,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="13" t="s">
         <v>130</v>
       </c>
@@ -3104,7 +3102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="13" t="s">
         <v>130</v>
       </c>
@@ -3159,7 +3157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="13" t="s">
         <v>130</v>
       </c>
@@ -3210,7 +3208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="13" t="s">
         <v>130</v>
       </c>
@@ -3264,7 +3262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="13" t="s">
         <v>130</v>
       </c>
@@ -3316,7 +3314,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="13" t="s">
         <v>130</v>
       </c>
@@ -3368,7 +3366,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="13" t="s">
         <v>130</v>
       </c>
@@ -3423,7 +3421,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="13" t="s">
         <v>130</v>
       </c>
@@ -3481,7 +3479,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="13" t="s">
         <v>130</v>
       </c>
@@ -3526,7 +3524,7 @@
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="13" t="s">
         <v>130</v>
       </c>
@@ -3586,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="13" t="s">
         <v>130</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="13" t="s">
         <v>130</v>
       </c>
@@ -3693,7 +3691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" s="13" t="s">
         <v>130</v>
       </c>
@@ -3744,7 +3742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="13" t="s">
         <v>130</v>
       </c>
@@ -3798,7 +3796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="13" t="s">
         <v>130</v>
       </c>
@@ -3850,7 +3848,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22">
       <c r="A33" s="13" t="s">
         <v>130</v>
       </c>
@@ -3902,7 +3900,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22">
       <c r="A34" s="13" t="s">
         <v>130</v>
       </c>
@@ -3957,7 +3955,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22">
       <c r="A35" s="13" t="s">
         <v>130</v>
       </c>
@@ -4015,7 +4013,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22">
       <c r="A36" s="13" t="s">
         <v>130</v>
       </c>
@@ -4060,7 +4058,7 @@
       <c r="U36" s="8"/>
       <c r="V36" s="8"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22">
       <c r="A37" s="13" t="s">
         <v>130</v>
       </c>
@@ -4120,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22">
       <c r="A38" s="13" t="s">
         <v>130</v>
       </c>
@@ -4172,7 +4170,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22">
       <c r="A39" s="13" t="s">
         <v>130</v>
       </c>
@@ -4227,7 +4225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22">
       <c r="A40" s="13" t="s">
         <v>130</v>
       </c>
@@ -4278,7 +4276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22">
       <c r="A41" s="13" t="s">
         <v>130</v>
       </c>
@@ -4332,7 +4330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22">
       <c r="A42" s="13" t="s">
         <v>130</v>
       </c>
@@ -4384,7 +4382,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22">
       <c r="A43" s="13" t="s">
         <v>130</v>
       </c>
@@ -4436,7 +4434,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22">
       <c r="A44" s="13" t="s">
         <v>130</v>
       </c>
@@ -4491,7 +4489,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22">
       <c r="A45" s="13" t="s">
         <v>130</v>
       </c>
@@ -4549,7 +4547,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22">
       <c r="A46" s="13" t="s">
         <v>130</v>
       </c>
@@ -4594,7 +4592,7 @@
       <c r="U46" s="8"/>
       <c r="V46" s="8"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22">
       <c r="A47" s="13" t="s">
         <v>130</v>
       </c>
@@ -4654,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22">
       <c r="A48" s="13" t="s">
         <v>130</v>
       </c>
@@ -4706,7 +4704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22">
       <c r="A49" s="13" t="s">
         <v>130</v>
       </c>
@@ -4761,7 +4759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22">
       <c r="A50" s="13" t="s">
         <v>130</v>
       </c>
@@ -4812,7 +4810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22">
       <c r="A51" s="13" t="s">
         <v>130</v>
       </c>
@@ -4866,7 +4864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22">
       <c r="A52" s="13" t="s">
         <v>130</v>
       </c>
@@ -4918,7 +4916,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22">
       <c r="A53" s="13" t="s">
         <v>130</v>
       </c>
@@ -4970,7 +4968,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22">
       <c r="A54" s="13" t="s">
         <v>130</v>
       </c>
@@ -5025,7 +5023,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22">
       <c r="A55" s="13" t="s">
         <v>130</v>
       </c>
@@ -5083,7 +5081,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22">
       <c r="A56" s="13" t="s">
         <v>130</v>
       </c>
@@ -5128,7 +5126,7 @@
       <c r="U56" s="8"/>
       <c r="V56" s="8"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22">
       <c r="A57" s="13" t="s">
         <v>130</v>
       </c>
@@ -5188,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22">
       <c r="A58" s="13" t="s">
         <v>130</v>
       </c>
@@ -5239,7 +5237,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22">
       <c r="A59" s="13" t="s">
         <v>130</v>
       </c>
@@ -5293,7 +5291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22">
       <c r="A60" s="13" t="s">
         <v>130</v>
       </c>
@@ -5344,7 +5342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22">
       <c r="A61" s="13" t="s">
         <v>130</v>
       </c>
@@ -5398,7 +5396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22">
       <c r="A62" s="13" t="s">
         <v>130</v>
       </c>
@@ -5450,7 +5448,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22">
       <c r="A63" s="13" t="s">
         <v>130</v>
       </c>
@@ -5502,7 +5500,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22">
       <c r="A64" s="13" t="s">
         <v>130</v>
       </c>
@@ -5557,7 +5555,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="A65" s="13" t="s">
         <v>130</v>
       </c>
@@ -5615,7 +5613,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="A66" s="13" t="s">
         <v>130</v>
       </c>
@@ -5660,7 +5658,7 @@
       <c r="U66" s="8"/>
       <c r="V66" s="8"/>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="A67" s="13" t="s">
         <v>130</v>
       </c>
@@ -5720,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="A68" s="13" t="s">
         <v>130</v>
       </c>
@@ -5772,7 +5770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="A69" s="13" t="s">
         <v>130</v>
       </c>
@@ -5827,7 +5825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="A70" s="13" t="s">
         <v>130</v>
       </c>
@@ -5878,7 +5876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="A71" s="13" t="s">
         <v>130</v>
       </c>
@@ -5932,7 +5930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="A72" s="13" t="s">
         <v>130</v>
       </c>
@@ -5984,7 +5982,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="A73" s="13" t="s">
         <v>130</v>
       </c>
@@ -6036,7 +6034,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="A74" s="13" t="s">
         <v>130</v>
       </c>
@@ -6091,7 +6089,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" s="13" t="s">
         <v>130</v>
       </c>
@@ -6149,7 +6147,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22">
       <c r="A76" s="13" t="s">
         <v>130</v>
       </c>
@@ -6194,7 +6192,7 @@
       <c r="U76" s="8"/>
       <c r="V76" s="8"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22">
       <c r="A77" s="13" t="s">
         <v>130</v>
       </c>
@@ -6254,7 +6252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22">
       <c r="A78" s="13" t="s">
         <v>130</v>
       </c>
@@ -6306,7 +6304,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22">
       <c r="A79" s="13" t="s">
         <v>130</v>
       </c>
@@ -6361,7 +6359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22">
       <c r="A80" s="13" t="s">
         <v>130</v>
       </c>
@@ -6412,7 +6410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22">
       <c r="A81" s="13" t="s">
         <v>130</v>
       </c>
@@ -6466,7 +6464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22">
       <c r="A82" s="13" t="s">
         <v>130</v>
       </c>
@@ -6518,7 +6516,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22">
       <c r="A83" s="13" t="s">
         <v>130</v>
       </c>
@@ -6570,7 +6568,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22">
       <c r="A84" s="13" t="s">
         <v>130</v>
       </c>
@@ -6625,7 +6623,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22">
       <c r="A85" s="13" t="s">
         <v>130</v>
       </c>
@@ -6683,7 +6681,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22">
       <c r="A86" s="13" t="s">
         <v>130</v>
       </c>
@@ -6728,7 +6726,7 @@
       <c r="U86" s="8"/>
       <c r="V86" s="8"/>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22">
       <c r="A87" s="13" t="s">
         <v>130</v>
       </c>
@@ -6788,7 +6786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22">
       <c r="A88" s="13" t="s">
         <v>130</v>
       </c>
@@ -6840,7 +6838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22">
       <c r="A89" s="13" t="s">
         <v>130</v>
       </c>
@@ -6895,7 +6893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22">
       <c r="A90" s="13" t="s">
         <v>130</v>
       </c>
@@ -6946,7 +6944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22">
       <c r="A91" s="13" t="s">
         <v>130</v>
       </c>
@@ -7000,7 +6998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22">
       <c r="A92" s="13" t="s">
         <v>130</v>
       </c>
@@ -7052,7 +7050,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22">
       <c r="A93" s="13" t="s">
         <v>130</v>
       </c>
@@ -7104,7 +7102,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22">
       <c r="A94" s="13" t="s">
         <v>130</v>
       </c>
@@ -7159,7 +7157,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22">
       <c r="A95" s="13" t="s">
         <v>130</v>
       </c>
@@ -7217,7 +7215,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22">
       <c r="A96" s="13" t="s">
         <v>130</v>
       </c>
@@ -7262,7 +7260,7 @@
       <c r="U96" s="8"/>
       <c r="V96" s="8"/>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22">
       <c r="A97" s="13" t="s">
         <v>130</v>
       </c>
@@ -7322,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22">
       <c r="A98" s="13" t="s">
         <v>130</v>
       </c>
@@ -7374,7 +7372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22">
       <c r="A99" s="13" t="s">
         <v>130</v>
       </c>
@@ -7429,7 +7427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22">
       <c r="A100" s="13" t="s">
         <v>130</v>
       </c>
@@ -7480,7 +7478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22">
       <c r="A101" s="13" t="s">
         <v>130</v>
       </c>
@@ -7534,7 +7532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22">
       <c r="A102" s="13" t="s">
         <v>130</v>
       </c>
@@ -7586,7 +7584,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22">
       <c r="A103" s="13" t="s">
         <v>130</v>
       </c>
@@ -7638,7 +7636,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22">
       <c r="A104" s="13" t="s">
         <v>130</v>
       </c>
@@ -7693,7 +7691,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22">
       <c r="A105" s="13" t="s">
         <v>130</v>
       </c>
@@ -7751,7 +7749,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22">
       <c r="A106" s="13" t="s">
         <v>130</v>
       </c>
@@ -7796,7 +7794,7 @@
       <c r="U106" s="8"/>
       <c r="V106" s="8"/>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22">
       <c r="A107" s="13" t="s">
         <v>130</v>
       </c>
@@ -7856,7 +7854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22">
       <c r="A108" s="13" t="s">
         <v>130</v>
       </c>
@@ -7908,7 +7906,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22">
       <c r="A109" s="13" t="s">
         <v>130</v>
       </c>
@@ -7963,7 +7961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22">
       <c r="A110" s="13" t="s">
         <v>130</v>
       </c>
@@ -8014,7 +8012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22">
       <c r="A111" s="13" t="s">
         <v>130</v>
       </c>
@@ -8068,7 +8066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22">
       <c r="A112" s="13" t="s">
         <v>130</v>
       </c>
@@ -8120,7 +8118,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22">
       <c r="A113" s="13" t="s">
         <v>130</v>
       </c>
@@ -8172,7 +8170,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22">
       <c r="A114" s="13" t="s">
         <v>130</v>
       </c>
@@ -8227,7 +8225,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22">
       <c r="A115" s="13" t="s">
         <v>130</v>
       </c>
@@ -8285,7 +8283,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22">
       <c r="A116" s="13" t="s">
         <v>130</v>
       </c>
@@ -8330,7 +8328,7 @@
       <c r="U116" s="8"/>
       <c r="V116" s="8"/>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22">
       <c r="A117" s="13" t="s">
         <v>130</v>
       </c>
@@ -8390,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22">
       <c r="A118" s="13" t="s">
         <v>130</v>
       </c>
@@ -8442,7 +8440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22">
       <c r="A119" s="13" t="s">
         <v>130</v>
       </c>
@@ -8497,7 +8495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22">
       <c r="A120" s="13" t="s">
         <v>130</v>
       </c>
@@ -8548,7 +8546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22">
       <c r="A121" s="13" t="s">
         <v>130</v>
       </c>
@@ -8602,7 +8600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22">
       <c r="A122" s="13" t="s">
         <v>130</v>
       </c>
@@ -8654,7 +8652,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22">
       <c r="A123" s="13" t="s">
         <v>130</v>
       </c>
@@ -8706,7 +8704,7 @@
         <v>54.650399999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22">
       <c r="A124" s="13" t="s">
         <v>130</v>
       </c>
@@ -8761,7 +8759,7 @@
         <v>30.956999999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22">
       <c r="A125" s="13" t="s">
         <v>130</v>
       </c>
@@ -8827,14 +8825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="14" style="8" customWidth="1"/>
@@ -8848,7 +8846,7 @@
     <col min="11" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" s="31" t="s">
         <v>363</v>
       </c>
@@ -8877,7 +8875,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="36.75" customHeight="1">
       <c r="B3" s="8" t="s">
         <v>357</v>
       </c>
@@ -8897,12 +8895,12 @@
         <v>361</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="36.75" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="36.75" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>349</v>
       </c>
@@ -8919,7 +8917,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="36.75" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>342</v>
       </c>
@@ -8936,7 +8934,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="36.75" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>69</v>
       </c>
@@ -8956,7 +8954,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="36.75" customHeight="1">
       <c r="B8" s="8" t="s">
         <v>373</v>
       </c>
@@ -8982,7 +8980,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="36.75" customHeight="1">
       <c r="B9" s="8" t="s">
         <v>119</v>
       </c>
@@ -9002,7 +9000,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="36.75" customHeight="1">
       <c r="B10" s="8" t="s">
         <v>379</v>
       </c>
@@ -9022,7 +9020,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="36.75" customHeight="1">
       <c r="B11" s="8" t="s">
         <v>338</v>
       </c>
@@ -9045,7 +9043,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="36.75" customHeight="1">
       <c r="B12" s="8" t="s">
         <v>419</v>
       </c>
@@ -9065,7 +9063,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="36.75" customHeight="1">
       <c r="B13" s="8" t="s">
         <v>353</v>
       </c>
@@ -9079,7 +9077,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="36.75" customHeight="1">
       <c r="B14" s="8" t="s">
         <v>389</v>
       </c>
@@ -9099,7 +9097,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="36.75" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>403</v>
       </c>
@@ -9116,7 +9114,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="36.75" customHeight="1">
       <c r="B16" s="8" t="s">
         <v>332</v>
       </c>
@@ -9139,7 +9137,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="36.75" customHeight="1">
       <c r="B17" s="8" t="s">
         <v>40</v>
       </c>
@@ -9156,7 +9154,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="36.75" customHeight="1">
       <c r="B18" s="8" t="s">
         <v>394</v>
       </c>
@@ -9179,7 +9177,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="36.75" customHeight="1">
       <c r="B19" s="8" t="s">
         <v>394</v>
       </c>
@@ -9202,21 +9200,21 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="21" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="22" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="23" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="24" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="25" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="26" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="27" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="28" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="29" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="30" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="31" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="32" spans="2:10" ht="42.75" customHeight="1"/>
+    <row r="33" ht="42.75" customHeight="1"/>
+    <row r="34" ht="42.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="B2:J2"/>
   <sortState ref="B3:J19">
@@ -9244,7 +9242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="B2:V39"/>
   <sheetViews>
@@ -9252,7 +9250,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.7109375" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
     <col min="2" max="9" width="9.85546875" style="5" customWidth="1"/>
@@ -9262,7 +9260,7 @@
     <col min="13" max="16384" width="6.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" s="8" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" s="8" customFormat="1" ht="62.25" customHeight="1">
       <c r="B2" s="8" t="s">
         <v>133</v>
       </c>
@@ -9320,7 +9318,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:22">
       <c r="B3" s="5" t="s">
         <v>208</v>
       </c>
@@ -9355,7 +9353,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:22">
       <c r="B4" s="5" t="s">
         <v>209</v>
       </c>
@@ -9390,7 +9388,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:22">
       <c r="B5" s="5" t="s">
         <v>210</v>
       </c>
@@ -9425,7 +9423,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:22">
       <c r="B6" s="5" t="s">
         <v>211</v>
       </c>
@@ -9460,7 +9458,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:22">
       <c r="B7" s="5" t="s">
         <v>134</v>
       </c>
@@ -9495,7 +9493,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:22">
       <c r="B8" s="5" t="s">
         <v>135</v>
       </c>
@@ -9530,7 +9528,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:22">
       <c r="B9" s="5" t="s">
         <v>212</v>
       </c>
@@ -9565,7 +9563,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:22">
       <c r="B10" s="5" t="s">
         <v>213</v>
       </c>
@@ -9600,7 +9598,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:22">
       <c r="B11" s="5" t="s">
         <v>214</v>
       </c>
@@ -9635,7 +9633,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:22">
       <c r="B12" s="5" t="s">
         <v>215</v>
       </c>
@@ -9670,7 +9668,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:22">
       <c r="B13" s="5" t="s">
         <v>136</v>
       </c>
@@ -9705,7 +9703,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:22">
       <c r="B14" s="5" t="s">
         <v>216</v>
       </c>
@@ -9740,7 +9738,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:22">
       <c r="B15" s="5" t="s">
         <v>217</v>
       </c>
@@ -9775,7 +9773,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:22">
       <c r="B16" s="5" t="s">
         <v>218</v>
       </c>
@@ -9810,46 +9808,46 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="10:10">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:10">
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="10:10">
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="10:10">
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:10">
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:10">
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="10:10">
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:10">
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="10:10">
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:10">
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:10">
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="10:10">
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:10">
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:10">
       <c r="J39" s="5"/>
     </row>
   </sheetData>
@@ -9859,7 +9857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:W16"/>
   <sheetViews>
@@ -9868,7 +9866,7 @@
       <selection pane="topRight" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
@@ -9882,7 +9880,7 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -9942,7 +9940,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -10010,7 +10008,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -10069,7 +10067,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -10137,7 +10135,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -10202,7 +10200,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -10270,7 +10268,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -10335,7 +10333,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>130</v>
       </c>
@@ -10401,7 +10399,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
@@ -10467,7 +10465,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
@@ -10533,7 +10531,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12" s="52" t="s">
         <v>130</v>
       </c>
@@ -10613,7 +10611,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
         <v>130</v>
       </c>
@@ -10679,7 +10677,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -10742,7 +10740,7 @@
         <v>81500</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
         <v>130</v>
       </c>
@@ -10805,7 +10803,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
@@ -10866,8 +10864,8 @@
         <v>0</v>
       </c>
       <c r="V16" s="50">
-        <f>91300-1500*10</f>
-        <v>76300</v>
+        <f>91300-1000*10</f>
+        <v>81300</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>425</v>
@@ -10881,7 +10879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -10889,7 +10887,7 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
@@ -10903,7 +10901,7 @@
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="8" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="8" customFormat="1" ht="45.75" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -10951,7 +10949,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="8" customFormat="1" ht="45.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -10998,7 +10996,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -11042,7 +11040,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -11089,7 +11087,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -11137,7 +11135,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -11185,16 +11183,16 @@
         <v>81200</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="B11" s="7"/>
     </row>
   </sheetData>
@@ -11204,7 +11202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -11212,7 +11210,7 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="16" customWidth="1"/>
@@ -11225,7 +11223,7 @@
     <col min="19" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1">
       <c r="A1" s="31" t="s">
         <v>24</v>
       </c>
@@ -11267,7 +11265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
@@ -11311,7 +11309,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="8" customFormat="1" ht="44.25" customHeight="1">
       <c r="A3" s="31" t="s">
         <v>141</v>
       </c>
@@ -11329,7 +11327,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="19" t="s">
         <v>26</v>
       </c>
@@ -11370,7 +11368,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>45</v>
       </c>
@@ -11414,7 +11412,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="5" t="s">
         <v>130</v>
       </c>
@@ -11464,7 +11462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:L46"/>
   <sheetViews>
@@ -11472,7 +11470,7 @@
       <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
@@ -11488,7 +11486,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="47.25" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -11521,7 +11519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="47.25" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -11559,7 +11557,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -11591,7 +11589,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -11629,7 +11627,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -11664,7 +11662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -11699,7 +11697,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -11734,7 +11732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>130</v>
       </c>
@@ -11772,7 +11770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
@@ -11810,7 +11808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
@@ -11848,7 +11846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -11886,7 +11884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>130</v>
       </c>
@@ -11924,103 +11922,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2">
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2">
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2">
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2">
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2">
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2">
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2">
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2">
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2">
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2">
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2">
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2">
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2">
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2">
       <c r="B41" s="7"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2">
       <c r="B42" s="7"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2">
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2">
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2">
       <c r="B45" s="7"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2">
       <c r="B46" s="7"/>
     </row>
   </sheetData>
@@ -12030,7 +12028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:J69"/>
   <sheetViews>
@@ -12038,7 +12036,7 @@
       <selection sqref="A1:XFD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
@@ -12061,7 +12059,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -12091,7 +12089,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -12123,7 +12121,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -12152,7 +12150,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -12184,7 +12182,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -12216,7 +12214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -12248,7 +12246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -12280,7 +12278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>130</v>
       </c>
@@ -12312,7 +12310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
@@ -12344,7 +12342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
@@ -12376,7 +12374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -12408,7 +12406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>130</v>
       </c>
@@ -12440,7 +12438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -12472,7 +12470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>130</v>
       </c>
@@ -12504,7 +12502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
@@ -12536,7 +12534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>130</v>
       </c>
@@ -12568,7 +12566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>130</v>
       </c>
@@ -12600,7 +12598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>130</v>
       </c>
@@ -12632,7 +12630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>130</v>
       </c>
@@ -12664,7 +12662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
@@ -12696,7 +12694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
@@ -12728,7 +12726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -12760,7 +12758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>130</v>
       </c>
@@ -12792,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
@@ -12824,7 +12822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
@@ -12856,7 +12854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>130</v>
       </c>
@@ -12888,7 +12886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
@@ -12920,7 +12918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -12952,7 +12950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>130</v>
       </c>
@@ -12984,7 +12982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -13016,7 +13014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>130</v>
       </c>
@@ -13048,7 +13046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>130</v>
       </c>
@@ -13080,52 +13078,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="B41" s="7"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2">
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2">
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2">
       <c r="B66" s="7"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2">
       <c r="B67" s="7"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2">
       <c r="B68" s="7"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2">
       <c r="B69" s="7"/>
     </row>
   </sheetData>
@@ -13135,7 +13133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1:K77"/>
   <sheetViews>
@@ -13143,7 +13141,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -13159,7 +13157,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -13180,7 +13178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="55.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -13206,12 +13204,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -13231,7 +13229,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -13260,7 +13258,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -13289,7 +13287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="B7" s="7"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -13297,7 +13295,7 @@
       <c r="H7" s="34"/>
       <c r="I7" s="35"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="B8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -13305,7 +13303,7 @@
       <c r="H8" s="34"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="B9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -13313,7 +13311,7 @@
       <c r="H9" s="34"/>
       <c r="I9" s="35"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="B10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -13321,7 +13319,7 @@
       <c r="H10" s="34"/>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="B11" s="7"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -13329,7 +13327,7 @@
       <c r="H11" s="34"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="B12" s="7"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -13337,7 +13335,7 @@
       <c r="H12" s="34"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="B13" s="7"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -13345,7 +13343,7 @@
       <c r="H13" s="34"/>
       <c r="I13" s="35"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="B14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -13353,7 +13351,7 @@
       <c r="H14" s="34"/>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="B15" s="7"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -13361,7 +13359,7 @@
       <c r="H15" s="34"/>
       <c r="I15" s="35"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="B16" s="7"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -13369,7 +13367,7 @@
       <c r="H16" s="34"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="B17" s="7"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -13377,7 +13375,7 @@
       <c r="H17" s="34"/>
       <c r="I17" s="35"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="B18" s="7"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -13385,7 +13383,7 @@
       <c r="H18" s="34"/>
       <c r="I18" s="35"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="B19" s="7"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -13393,7 +13391,7 @@
       <c r="H19" s="34"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="B20" s="7"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -13401,314 +13399,314 @@
       <c r="H20" s="34"/>
       <c r="I20" s="35"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="H21" s="34"/>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="H22" s="34"/>
       <c r="I22" s="35"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="35"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9">
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="H24" s="34"/>
       <c r="I24" s="35"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9">
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="35"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9">
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="H26" s="34"/>
       <c r="I26" s="35"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9">
       <c r="B28" s="7"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9">
       <c r="B29" s="7"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="B30" s="7"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="B31" s="7"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="B32" s="7"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6">
       <c r="B33" s="7"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6">
       <c r="B34" s="7"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6">
       <c r="B35" s="7"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6">
       <c r="B36" s="7"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6">
       <c r="B37" s="7"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6">
       <c r="B38" s="7"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6">
       <c r="B39" s="7"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6">
       <c r="B40" s="7"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6">
       <c r="B41" s="7"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6">
       <c r="B42" s="7"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6">
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6">
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6">
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6">
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6">
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6">
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:6">
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:6">
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:6">
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
     </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:6">
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:6">
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
     </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:6">
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:6">
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:6">
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:6">
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
     </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:6">
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
     </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:6">
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:6">
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
     </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:6">
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
     </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:6">
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
     </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:6">
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:6">
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
     </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:6">
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
     </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:6">
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:6">
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
     </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:6">
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
     </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:6">
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
     </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:6">
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
     </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:6">
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:6">
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
     </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:6">
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
     </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:6">
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
     </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:6">
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:6">
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:6">
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
@@ -13719,7 +13717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle9"/>
   <dimension ref="A1:W12"/>
   <sheetViews>
@@ -13728,7 +13726,7 @@
       <selection pane="topRight" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11" style="1" customWidth="1"/>
@@ -13751,7 +13749,7 @@
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="8" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="8" customFormat="1" ht="66.75" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -13777,7 +13775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="8" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="8" customFormat="1" ht="66.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -13818,7 +13816,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -13847,7 +13845,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -13898,7 +13896,7 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -13922,7 +13920,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -13946,7 +13944,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -13981,7 +13979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>130</v>
       </c>
@@ -14016,7 +14014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
@@ -14051,7 +14049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
@@ -14086,7 +14084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="F12" s="20"/>
     </row>
   </sheetData>

</xml_diff>